<commit_message>
Worked on the Effects doc. + Cleaned the Vampire skills doc.
</commit_message>
<xml_diff>
--- a/GameDesign/Class/_Done/9-Vampire/Documentation/VampireSkills.xlsx
+++ b/GameDesign/Class/_Done/9-Vampire/Documentation/VampireSkills.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="843" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="1-Bite" sheetId="1" r:id="rId1"/>
@@ -33,41 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="105">
-  <si>
-    <t>[[AP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[MP: 0 ]]</t>
-  </si>
-  <si>
-    <t>[[Range: 0-0 ]]</t>
-  </si>
-  <si>
-    <t>[[Cast in straight line: - ]]</t>
-  </si>
-  <si>
-    <t>[[Modifiable range: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of casts per turn: - ]]</t>
-  </si>
-  <si>
-    <t>[[Number of cast per turn per target: - ]]</t>
-  </si>
-  <si>
-    <t>[[Max effect accumulation: - ]]</t>
-  </si>
-  <si>
-    <t>[[Line of sight: - ]]</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="85">
   <si>
     <t>Additional Info</t>
   </si>
   <si>
-    <t>[[Number of turns between two casts: -  ]]</t>
-  </si>
-  <si>
     <t>Bite</t>
   </si>
   <si>
@@ -110,24 +80,9 @@
     <t>[[Cast in straight line: No ]]</t>
   </si>
   <si>
-    <t>Teleport the caster at the targeted cell.</t>
-  </si>
-  <si>
-    <t>[[Melee Invulnerable]] (1 turn)</t>
-  </si>
-  <si>
-    <t>Automatically end turn.</t>
-  </si>
-  <si>
     <t>[[Number of turns between two casts: 5 ]]</t>
   </si>
   <si>
-    <t>Teleports to the targeted cell and become invulnarable from melee damage.                                                                                             End the turn.</t>
-  </si>
-  <si>
-    <t>Effect name: ''Melee Invulnerable''.</t>
-  </si>
-  <si>
     <t>Shadow Control</t>
   </si>
   <si>
@@ -143,15 +98,6 @@
     <t>Blood Transfusion</t>
   </si>
   <si>
-    <t>Caster: [[-10% caster HP]]</t>
-  </si>
-  <si>
-    <t>Caster: [[-10% caster Max HP]]</t>
-  </si>
-  <si>
-    <t>Target: [[+20% caster Max HP]]</t>
-  </si>
-  <si>
     <t>[[Number of casts per turn: 1 ]]</t>
   </si>
   <si>
@@ -164,27 +110,15 @@
     <t>[[Line of sight: Yes ]]</t>
   </si>
   <si>
-    <t>Effect name: ''Void''.</t>
-  </si>
-  <si>
     <t>Heal the target depending of the caster Max HP.                              The caster life expectancy is reduced.</t>
   </si>
   <si>
     <t>Vampire Mark</t>
   </si>
   <si>
-    <t>Effect name: ''Vampire Mark''.</t>
-  </si>
-  <si>
-    <t>Target: [[''Vampire Mark'' effect]] (3 turns)</t>
-  </si>
-  <si>
     <t>Else:</t>
   </si>
   <si>
-    <t>[[Max effect accumulation: 3 ]]</t>
-  </si>
-  <si>
     <t>Shadow Spear</t>
   </si>
   <si>
@@ -194,45 +128,21 @@
     <t>[[Damage:  30-60 dark ]]</t>
   </si>
   <si>
-    <t>[[Damage:  20 dark ]] (2 turns)</t>
-  </si>
-  <si>
-    <t>Push 1 cell in the opposite direction of the spell cast point.</t>
-  </si>
-  <si>
     <t>Inflicts Dark-type damage and Dark-type poison damage.                                                                                           Push the target.</t>
   </si>
   <si>
-    <t>Effect name: ''Poison''.</t>
-  </si>
-  <si>
     <t>Coffin</t>
   </si>
   <si>
-    <t>Target: [[Invulnerable]] (1 turn)</t>
-  </si>
-  <si>
-    <t>Effect name: ''Invulnerable''.</t>
-  </si>
-  <si>
     <t>[[AP: 6 ]]</t>
   </si>
   <si>
-    <t>Self target:    End turn.</t>
-  </si>
-  <si>
-    <t>Other target: Skip next turn (1 turn)</t>
-  </si>
-  <si>
     <t>[[Range: 0-2 ]]</t>
   </si>
   <si>
     <t>[[Number of turns between two casts: 6 ]]</t>
   </si>
   <si>
-    <t>[[Max effect accumulation: 1 ]]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Make the target invulnarable and skip his turn.   </t>
   </si>
   <si>
@@ -242,15 +152,6 @@
     <t>[[Number of turns between two casts: 5  ]]</t>
   </si>
   <si>
-    <t>[[Aura of Terror]] (1 turn)</t>
-  </si>
-  <si>
-    <t>Effect name: ''Aura of Terror''.</t>
-  </si>
-  <si>
-    <t>Entity adjacent of the target: Push the target by 1 cell. (1 turn)</t>
-  </si>
-  <si>
     <t>All the adjacent entity of the target are pushed away.                               When the entity whit ''Aura of Terror'' move, all the entity adjacent of him get pushed away.                                                                       When an entity move on a cell adjacent of the entity whit ''Aura of Terror'', the entity is pushed away.</t>
   </si>
   <si>
@@ -260,101 +161,364 @@
     <t>[[Number of turns between two casts: 2 ]]</t>
   </si>
   <si>
-    <t>Summoned whit the ''Zombification'' effect. (00 turns)</t>
-  </si>
-  <si>
-    <t>Can summon 1 Ghoul + number of allies player K/O</t>
-  </si>
-  <si>
-    <t>Effect name: ''Zombification''.</t>
-  </si>
-  <si>
-    <t>Inflicts Earth-type damage and give poisons that inflicts Dark-type damage.</t>
-  </si>
-  <si>
-    <t>[[Max effect accumulation: 2 ]]</t>
-  </si>
-  <si>
     <t>Ghoul skills</t>
   </si>
   <si>
     <t>Infected Claw</t>
   </si>
   <si>
-    <t>[[Damage: 5-10 earth ]]                                                      [[Damage: 10 dark ]] (2 turns)</t>
-  </si>
-  <si>
     <t>Zombification</t>
   </si>
   <si>
     <t>[[AP: 2 ]]</t>
   </si>
   <si>
-    <t>Summons a ''Ghoul'' [[20% summoner HP, 5 AP, 3 MP, 40% earth resistence, -10% fire resistence, -20% water resistence, 10% air resistence, -50% light resistence, 50% dark resistence]]</t>
-  </si>
-  <si>
     <t>Temporarily give ''Zombification'' effect to the target.</t>
   </si>
   <si>
-    <t>Give the ''Zombification'' effect. (1 turn)</t>
-  </si>
-  <si>
-    <t>Summons a Ghoul which can zombify and poison.                                                                                                         Can only be used if the caster is not under the Treason effect.</t>
-  </si>
-  <si>
     <t>Red Moon</t>
   </si>
   <si>
     <t>[[Area of effect: - All the map ]]</t>
   </si>
   <si>
-    <t>Effect name: ''Red Moon''.</t>
-  </si>
-  <si>
-    <t>[[''Red Moon'' effect]] (1 turn)</t>
-  </si>
-  <si>
     <t>Steal Dark-type health.                                                                More effective on allies player</t>
   </si>
   <si>
-    <t>Life steal skills ratio go from 50% to 100% steal.</t>
-  </si>
-  <si>
-    <t>If self HP &gt; 25% max HP</t>
-  </si>
-  <si>
-    <t>If entities under ''Vampire Mark''</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Self: [[HP - 25% max HP ]]</t>
-  </si>
-  <si>
     <t>Allies:     [[Damage:  50-55 fire steal ]]</t>
   </si>
   <si>
     <t>Enemies: [[Damage:  40-45 fire steal ]]</t>
   </si>
   <si>
-    <t xml:space="preserve">    Entities: [[Damage:  25 fire steal]]</t>
-  </si>
-  <si>
-    <t>Poisons that inflicts Fire-type steal damage.                                                   The poison is stronger if the caster is under ''Blood Moon'' effect.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Target: [[Damage:  30 fire steal ]] (3 turns)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Target: [[Damage:  20 fire steal ]] (3 turns)</t>
-  </si>
-  <si>
-    <t>If under "Red Moon" effect:</t>
+    <t>End current turn.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Invulnerable (Melee)]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>Teleport on the targeted cell.</t>
+  </si>
+  <si>
+    <t>Teleports on the targeted cell and become invulnarable from melee damage.                                                                                             End the turn.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caster: </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Void]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +10 levels (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>[[Heal 20% of caster HP]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    [[Damage 10% of caster HP]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Poison]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +20 levels (2 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Push the target by 1 cell.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Invulnerable]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>If self targeting:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    End current turn.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Skip]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Aura of Terror]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Summons a Ghoul which can zombify and poison.                                                One Ghoul can be summoned by default, one extra Ghoul can be summoned per the amount of allied player K/O.                                    </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Zombification]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (00 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>Inflicts Ground-type damage and give poisons that inflicts Dark-type damage.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Poison]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +10 levels (2 turns)                                                             Enemy: [[Damage: 5-10 ground ]]     </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Zombification]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>If self HP &gt; 25% Max HP:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Self: [[Damage: 25% HP]]</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Red Moon]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    Entity: [[Damage: 25 fire steal]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If entity have </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vampire Mark]]</t>
+    </r>
+  </si>
+  <si>
+    <t>[[Range: 0 ]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poisons that inflicts Fire-type steal damage. </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Vampire Mark]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +20 levels (3 turns)</t>
+    </r>
+  </si>
+  <si>
+    <t>[[Number of turns between two casts: 7 ]]</t>
+  </si>
+  <si>
+    <t>[[AP: 1 ]]</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Self: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t>[[Speed]]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial Black"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> +2 levels (1 turn)</t>
+    </r>
+  </si>
+  <si>
+    <t>Summons a ''Ghoul'' [[20% summoner HP, 5 AP, 3 MP, 30% ground resistence, 50% fire resistence, -20% water resistence, 20% wind resistence, -50% light resistence, 50% dark resistence]]</t>
+  </si>
+  <si>
+    <t>Every skills can steal life, and the skills that were already stealing life can now steal even more life.                                                     The caster speed increase.                                                                             Steal Fire-type health to every entity whit the ''Vampire Mark''                    Carfull! Can be dangerous for the caster if his HP is too high.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,6 +557,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Arial Black"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -500,7 +670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -539,6 +709,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -876,7 +1047,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -888,7 +1059,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>93</v>
+        <v>49</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -900,14 +1071,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -919,7 +1090,7 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -931,14 +1102,14 @@
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -950,7 +1121,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -962,14 +1133,14 @@
     <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
       <c r="C17" s="10" t="s">
-        <v>99</v>
+        <v>51</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="D18" s="1"/>
     </row>
@@ -987,7 +1158,7 @@
     <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B22" s="1"/>
       <c r="C22" s="4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -1014,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D35"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1208,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1046,9 +1217,11 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
-      <c r="C5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>84</v>
+      </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -1059,181 +1232,132 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>1</v>
+        <v>77</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
-      <c r="C9" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C9" s="2"/>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
-      <c r="C11" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
-      <c r="C13" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="C13" s="2"/>
       <c r="D13" s="1"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
-      <c r="C15" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="1"/>
-      <c r="C16" s="6" t="s">
-        <v>7</v>
+      <c r="C16" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="11" t="s">
+        <v>82</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>5</v>
+      <c r="C18" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
-        <v>6</v>
+      <c r="C19" s="12" t="s">
+        <v>75</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="2"/>
+      <c r="C20" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="2" t="s">
-        <v>90</v>
+      <c r="C21" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B23" s="1"/>
-      <c r="C23" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="12" t="s">
-        <v>97</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="10" t="s">
-        <v>92</v>
+      <c r="C25" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="10" t="s">
-        <v>94</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="11" t="s">
-        <v>96</v>
-      </c>
+      <c r="C27" s="8"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B32" s="1"/>
-      <c r="C32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B34" s="1"/>
-      <c r="C34" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="5"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1245,8 +1369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1390,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1278,7 +1402,7 @@
     <row r="5" spans="2:4" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1290,21 +1414,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1316,21 +1440,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1342,7 +1466,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1354,7 +1478,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1366,21 +1490,21 @@
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="10" t="s">
-        <v>25</v>
+        <v>54</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="10" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
       <c r="C21" s="10" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1398,7 +1522,7 @@
     <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -1409,9 +1533,7 @@
     </row>
     <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="C27" s="8"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -1450,7 +1572,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1462,7 +1584,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1474,21 +1596,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -1500,21 +1622,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -1526,7 +1648,7 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -1538,7 +1660,7 @@
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
     </row>
@@ -1550,7 +1672,7 @@
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
       <c r="C19" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D19" s="1"/>
     </row>
@@ -1568,7 +1690,7 @@
     <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
       <c r="C23" s="4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -1595,10 +1717,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+  <dimension ref="B2:D28"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1618,7 +1740,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1630,7 +1752,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1642,14 +1764,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1661,21 +1783,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1687,7 +1809,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -1699,7 +1821,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -1708,61 +1830,66 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
-      <c r="C18" s="11" t="s">
-        <v>36</v>
+      <c r="C18" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="12" t="s">
-        <v>37</v>
+      <c r="C19" s="11" t="s">
+        <v>56</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
-      <c r="C20" s="10" t="s">
-        <v>38</v>
+      <c r="C20" s="13" t="s">
+        <v>59</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="C21" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="8" t="s">
-        <v>43</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="1"/>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1772,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D32"/>
+  <dimension ref="B2:D26"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1795,7 +1922,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -1804,10 +1931,10 @@
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>101</v>
+        <v>78</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1819,14 +1946,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -1838,21 +1965,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -1863,116 +1990,74 @@
     </row>
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
-      <c r="C14" s="6" t="s">
-        <v>49</v>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
-        <v>17</v>
+      <c r="C19" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B21" s="1"/>
-      <c r="C21" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
-      <c r="C22" s="11" t="s">
-        <v>104</v>
-      </c>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="13" t="s">
-        <v>102</v>
+      <c r="C23" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
-      <c r="C24" s="13" t="s">
-        <v>48</v>
-      </c>
+      <c r="C24" s="1"/>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B25" s="1"/>
-      <c r="C25" s="12" t="s">
-        <v>103</v>
-      </c>
+      <c r="C25" s="8"/>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="B29" s="1"/>
-      <c r="C29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B31" s="1"/>
-      <c r="C31" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="5"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1984,8 +2069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D27"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2005,7 +2090,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2017,7 +2102,7 @@
     <row r="5" spans="2:4" ht="39" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2029,14 +2114,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2048,21 +2133,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2074,7 +2159,7 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -2086,7 +2171,7 @@
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2098,21 +2183,21 @@
     <row r="18" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="1"/>
       <c r="C18" s="10" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="10" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="10" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -2130,7 +2215,7 @@
     <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B24" s="1"/>
       <c r="C24" s="4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -2141,9 +2226,7 @@
     </row>
     <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B26" s="1"/>
-      <c r="C26" s="8" t="s">
-        <v>56</v>
-      </c>
+      <c r="C26" s="8"/>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -2159,10 +2242,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D29"/>
+  <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2182,7 +2265,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2194,7 +2277,7 @@
     <row r="5" spans="2:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2206,21 +2289,21 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -2232,21 +2315,21 @@
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -2258,89 +2341,94 @@
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="C16" s="2"/>
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
-      <c r="C18" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="C19" s="20" t="s">
+        <v>62</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B20" s="1"/>
       <c r="C20" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="12" t="s">
-        <v>62</v>
+      <c r="C21" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B22" s="1"/>
-      <c r="C22" s="10" t="s">
-        <v>58</v>
+      <c r="C22" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
-      <c r="C26" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="C27" s="4" t="s">
+        <v>0</v>
+      </c>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
-      <c r="C28" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2350,10 +2438,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+  <dimension ref="B2:D25"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,7 +2461,7 @@
     <row r="3" spans="2:4" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -2385,7 +2473,7 @@
     <row r="5" spans="2:4" ht="97.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -2397,14 +2485,14 @@
     <row r="7" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -2416,21 +2504,21 @@
     <row r="10" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B10" s="1"/>
       <c r="C10" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -2442,82 +2530,66 @@
     <row r="14" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
-        <v>68</v>
+        <v>38</v>
       </c>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
-      <c r="C15" s="6" t="s">
-        <v>65</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B16" s="1"/>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
-      <c r="C17" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
+      <c r="C18" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
-      <c r="C19" s="2" t="s">
-        <v>69</v>
-      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B20" s="1"/>
-      <c r="C20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
+    <row r="20" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="1"/>
+      <c r="C22" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1"/>
+    </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B24" s="1"/>
-      <c r="C24" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="C24" s="8"/>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="2:4" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="B26" s="1"/>
-      <c r="C26" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="5"/>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2527,7 +2599,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H53"/>
+  <dimension ref="B1:H51"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
@@ -2545,7 +2617,7 @@
     <row r="1" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
       <c r="G1" s="15" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="H1" s="1"/>
     </row>
@@ -2560,12 +2632,12 @@
     <row r="3" spans="2:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="7" t="s">
-        <v>73</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="7" t="s">
-        <v>81</v>
+        <v>43</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -2577,15 +2649,15 @@
       <c r="G4" s="3"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="2:8" ht="39" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" ht="58.5" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="9" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="D5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="9" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -2600,19 +2672,19 @@
     <row r="7" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="D7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B8" s="1"/>
       <c r="C8" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1"/>
       <c r="F8" s="1"/>
@@ -2622,12 +2694,12 @@
     <row r="9" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B9" s="1"/>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -2642,19 +2714,19 @@
     <row r="11" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B11" s="1"/>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B12" s="1"/>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1"/>
       <c r="F12" s="1"/>
@@ -2664,13 +2736,11 @@
     <row r="13" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="6" t="s">
-        <v>79</v>
-      </c>
+      <c r="G13" s="6"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
@@ -2684,7 +2754,7 @@
     <row r="15" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="D15" s="1"/>
       <c r="F15" s="1"/>
@@ -2702,12 +2772,12 @@
     <row r="17" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B17" s="1"/>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -2722,19 +2792,19 @@
     <row r="19" spans="2:8" ht="59.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B19" s="1"/>
       <c r="C19" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="17" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B20" s="1"/>
       <c r="C20" s="10" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1"/>
       <c r="F20" s="1"/>
@@ -2743,9 +2813,7 @@
     </row>
     <row r="21" spans="2:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="B21" s="1"/>
-      <c r="C21" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="C21" s="2"/>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -2759,7 +2827,7 @@
     <row r="23" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="F23" s="1"/>
       <c r="G23" s="4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -2774,7 +2842,7 @@
     <row r="25" spans="2:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="B25" s="1"/>
       <c r="C25" s="4" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D25" s="1"/>
       <c r="F25" s="1"/>
@@ -2791,9 +2859,7 @@
     </row>
     <row r="27" spans="2:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B27" s="1"/>
-      <c r="C27" s="8" t="s">
-        <v>77</v>
-      </c>
+      <c r="C27" s="8"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2809,7 +2875,7 @@
     <row r="30" spans="2:8" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F30" s="1"/>
       <c r="G30" s="15" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="H30" s="1"/>
     </row>
@@ -2821,7 +2887,7 @@
     <row r="32" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="F32" s="1"/>
       <c r="G32" s="7" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -2833,7 +2899,7 @@
     <row r="34" spans="6:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="F34" s="1"/>
       <c r="G34" s="16" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="H34" s="1"/>
     </row>
@@ -2845,7 +2911,7 @@
     <row r="36" spans="6:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="F36" s="1"/>
       <c r="G36" s="2" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="H36" s="1"/>
     </row>
@@ -2857,7 +2923,7 @@
     <row r="38" spans="6:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="F38" s="1"/>
       <c r="G38" s="2" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="H38" s="1"/>
     </row>
@@ -2869,7 +2935,7 @@
     <row r="40" spans="6:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="F40" s="1"/>
       <c r="G40" s="2" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H40" s="1"/>
     </row>
@@ -2880,20 +2946,20 @@
     </row>
     <row r="42" spans="6:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="F42" s="1"/>
-      <c r="G42" s="6" t="s">
-        <v>65</v>
+      <c r="G42" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="6:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="43" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F43" s="1"/>
-      <c r="G43" s="2"/>
+      <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="6:8" ht="19.5" x14ac:dyDescent="0.4">
+    <row r="44" spans="6:8" ht="19.5" x14ac:dyDescent="0.25">
       <c r="F44" s="1"/>
-      <c r="G44" s="2" t="s">
-        <v>17</v>
+      <c r="G44" s="17" t="s">
+        <v>71</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -2902,46 +2968,32 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="6:8" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="F46" s="1"/>
-      <c r="G46" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="H46" s="1"/>
-    </row>
     <row r="47" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
+    <row r="48" spans="6:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="F48" s="1"/>
+      <c r="G48" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1"/>
+    </row>
     <row r="49" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" spans="6:8" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="50" spans="6:8" ht="19.5" x14ac:dyDescent="0.4">
       <c r="F50" s="1"/>
-      <c r="G50" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="G50" s="8"/>
       <c r="H50" s="1"/>
     </row>
     <row r="51" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="6:8" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="F52" s="1"/>
-      <c r="G52" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="6:8" x14ac:dyDescent="0.25">
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="18"/>
+      <c r="H51" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>